<commit_message>
edite import file persons-excel
</commit_message>
<xml_diff>
--- a/public_html/imports/persons-import.xlsx
+++ b/public_html/imports/persons-import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF3DA70-7621-4A2B-8D99-8DA2BDA0C770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB30F02D-572C-4327-9698-AF7304EF06A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
-  <si>
-    <t>کد</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>نام مستعار(الزامی)</t>
   </si>
@@ -84,7 +81,7 @@
     <t>آدرس</t>
   </si>
   <si>
-    <t>دسترسی سریع ۱ فعال</t>
+    <t>دسترسی سریع (۱) فعال</t>
   </si>
 </sst>
 </file>
@@ -108,12 +105,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -128,12 +131,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -416,80 +416,79 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" customWidth="1"/>
     <col min="13" max="13" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>